<commit_message>
Remove local tesseract path for cloud
</commit_message>
<xml_diff>
--- a/suppliers.xlsx
+++ b/suppliers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash Rathod\Desktop\iso_automation\iso_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF70D79E-2492-4C94-856A-E523253A3ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5092CA81-4AED-46C0-8A06-C61DE73761E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5E206C4F-FE7F-4599-9462-21947E0F5430}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Supplier Number</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>extra</t>
+  </si>
+  <si>
+    <t>after</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA197A9-5699-4E90-98A2-C23EF9855D0F}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,12 +523,27 @@
         <v>97435437782</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>1005</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>97435437782</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{B22C86B4-4924-43C0-B95D-343DD5FB7C42}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{6AE9A7BC-17E0-432E-9976-74ACB8DEFB6E}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{49E5E5A2-8755-4083-B93A-DADE56B22422}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{AF453FFF-DD6E-4E17-AB75-CB632EC01B1B}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{987A2313-80AB-4630-BEEB-68B53CC1EBB0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>